<commit_message>
Obteniendo los datos meteorológicos de todas las islas
</commit_message>
<xml_diff>
--- a/data/Inicial/datos_meteorologicos/Diccionario datos/estaciones.xlsx
+++ b/data/Inicial/datos_meteorologicos/Diccionario datos/estaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\TFM\data\Inicial\datos_meteorologicos\Diccionario datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\TFM\data\Inicial\datos_meteorologicos\Diccionario datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD7A81F-D52B-40CD-A30B-EECB04BF0847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A05C0A-2695-4656-912E-D004C2B89E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="537">
   <si>
     <t>latitud</t>
   </si>
@@ -715,6 +715,51 @@
     <t>162420W</t>
   </si>
   <si>
+    <t>282214N</t>
+  </si>
+  <si>
+    <t>525</t>
+  </si>
+  <si>
+    <t>C436L</t>
+  </si>
+  <si>
+    <t>CITFAGRO_96_ARAYA</t>
+  </si>
+  <si>
+    <t>162351W</t>
+  </si>
+  <si>
+    <t>281611N</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>C437E</t>
+  </si>
+  <si>
+    <t>CITFAGRO_81_MENA</t>
+  </si>
+  <si>
+    <t>162511W</t>
+  </si>
+  <si>
+    <t>282132N</t>
+  </si>
+  <si>
+    <t>463</t>
+  </si>
+  <si>
+    <t>C438N</t>
+  </si>
+  <si>
+    <t>CANDELARIA</t>
+  </si>
+  <si>
+    <t>162405W</t>
+  </si>
+  <si>
     <t>281906N</t>
   </si>
   <si>
@@ -733,6 +778,21 @@
     <t>162256W</t>
   </si>
   <si>
+    <t>283136N</t>
+  </si>
+  <si>
+    <t>868</t>
+  </si>
+  <si>
+    <t>C446G</t>
+  </si>
+  <si>
+    <t>SAN CRISTÓBAL DE LA LAGUNA,LLANO DE LOS LOROS</t>
+  </si>
+  <si>
+    <t>161650W</t>
+  </si>
+  <si>
     <t>282839N</t>
   </si>
   <si>
@@ -751,6 +811,21 @@
     <t>161946W</t>
   </si>
   <si>
+    <t>282745N</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>C448C</t>
+  </si>
+  <si>
+    <t>CITFAGRO_92_SANTACRUZ</t>
+  </si>
+  <si>
+    <t>161624W</t>
+  </si>
+  <si>
     <t>282748N</t>
   </si>
   <si>
@@ -769,6 +844,171 @@
     <t>161519W</t>
   </si>
   <si>
+    <t>283029N</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>C449F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANAGA </t>
+  </si>
+  <si>
+    <t>161144W</t>
+  </si>
+  <si>
+    <t>283336N</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>C449Q</t>
+  </si>
+  <si>
+    <t>CITFAGRO_97_TAGANANA</t>
+  </si>
+  <si>
+    <t>161341W</t>
+  </si>
+  <si>
+    <t>282341N</t>
+  </si>
+  <si>
+    <t>1744</t>
+  </si>
+  <si>
+    <t>C453I</t>
+  </si>
+  <si>
+    <t>CITFAGRO_88_GAITERO</t>
+  </si>
+  <si>
+    <t>162600W</t>
+  </si>
+  <si>
+    <t>282142N</t>
+  </si>
+  <si>
+    <t>1065</t>
+  </si>
+  <si>
+    <t>C455M</t>
+  </si>
+  <si>
+    <t>CITFAGRO_87_AGUAMANSA</t>
+  </si>
+  <si>
+    <t>162949W</t>
+  </si>
+  <si>
+    <t>282714N</t>
+  </si>
+  <si>
+    <t>922</t>
+  </si>
+  <si>
+    <t>C456E</t>
+  </si>
+  <si>
+    <t>CITFAGRO_10_RAVELO</t>
+  </si>
+  <si>
+    <t>162431W</t>
+  </si>
+  <si>
+    <t>282141N</t>
+  </si>
+  <si>
+    <t>906</t>
+  </si>
+  <si>
+    <t>C456P</t>
+  </si>
+  <si>
+    <t>CITFAGRO_70_BENIJO</t>
+  </si>
+  <si>
+    <t>163248W</t>
+  </si>
+  <si>
+    <t>282222N</t>
+  </si>
+  <si>
+    <t>551</t>
+  </si>
+  <si>
+    <t>C456R</t>
+  </si>
+  <si>
+    <t>CITFAGRO_69_SUERTE</t>
+  </si>
+  <si>
+    <t>163231W</t>
+  </si>
+  <si>
+    <t>282658N</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>C457E</t>
+  </si>
+  <si>
+    <t>CITFAGRO_67_MATANZA</t>
+  </si>
+  <si>
+    <t>162617W</t>
+  </si>
+  <si>
+    <t>282605N</t>
+  </si>
+  <si>
+    <t>567</t>
+  </si>
+  <si>
+    <t>C457I</t>
+  </si>
+  <si>
+    <t>LA VICTORIA DE ACENTEJO</t>
+  </si>
+  <si>
+    <t>162717W</t>
+  </si>
+  <si>
+    <t>282947N</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>C458A</t>
+  </si>
+  <si>
+    <t>TACORONTE</t>
+  </si>
+  <si>
+    <t>162512W</t>
+  </si>
+  <si>
+    <t>282207N</t>
+  </si>
+  <si>
+    <t>595</t>
+  </si>
+  <si>
+    <t>C458U</t>
+  </si>
+  <si>
+    <t>CITFAGRO_71_PALOB</t>
+  </si>
+  <si>
+    <t>163441W</t>
+  </si>
+  <si>
     <t>282505N</t>
   </si>
   <si>
@@ -784,6 +1024,126 @@
     <t>163253W</t>
   </si>
   <si>
+    <t>282021N</t>
+  </si>
+  <si>
+    <t>878</t>
+  </si>
+  <si>
+    <t>C466O</t>
+  </si>
+  <si>
+    <t>CITFAGRO_91_CUBO</t>
+  </si>
+  <si>
+    <t>164740W</t>
+  </si>
+  <si>
+    <t>282112N</t>
+  </si>
+  <si>
+    <t>C467I</t>
+  </si>
+  <si>
+    <t>CITFAGRO_73_REDON</t>
+  </si>
+  <si>
+    <t>164230W</t>
+  </si>
+  <si>
+    <t>282201N</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>C468I</t>
+  </si>
+  <si>
+    <t>CITFAGRO_98_ELDRAGO</t>
+  </si>
+  <si>
+    <t>164320W</t>
+  </si>
+  <si>
+    <t>282125N</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>C468O</t>
+  </si>
+  <si>
+    <t>CITFAGRO_62_TRIGO</t>
+  </si>
+  <si>
+    <t>164805W</t>
+  </si>
+  <si>
+    <t>282223N</t>
+  </si>
+  <si>
+    <t>677</t>
+  </si>
+  <si>
+    <t>C468X</t>
+  </si>
+  <si>
+    <t>SAN JUAN DE LA RAMBLA</t>
+  </si>
+  <si>
+    <t>163733W</t>
+  </si>
+  <si>
+    <t>275838N</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>C611E</t>
+  </si>
+  <si>
+    <t>VEGA DE SAN MATEO</t>
+  </si>
+  <si>
+    <t>153502W</t>
+  </si>
+  <si>
+    <t>280025N</t>
+  </si>
+  <si>
+    <t>1514</t>
+  </si>
+  <si>
+    <t>C612F</t>
+  </si>
+  <si>
+    <t>TEJEDA, CRUZ DE TEJEDA</t>
+  </si>
+  <si>
+    <t>153556W</t>
+  </si>
+  <si>
+    <t>275943N</t>
+  </si>
+  <si>
+    <t>1060</t>
+  </si>
+  <si>
+    <t>C614H</t>
+  </si>
+  <si>
+    <t>TEJEDA</t>
+  </si>
+  <si>
+    <t>60038</t>
+  </si>
+  <si>
+    <t>153657W</t>
+  </si>
+  <si>
     <t>280003N</t>
   </si>
   <si>
@@ -802,6 +1162,90 @@
     <t>154850W</t>
   </si>
   <si>
+    <t>280604N</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>C619X</t>
+  </si>
+  <si>
+    <t>AGAETE</t>
+  </si>
+  <si>
+    <t>154246W</t>
+  </si>
+  <si>
+    <t>280004N</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>C619Y</t>
+  </si>
+  <si>
+    <t>154827W</t>
+  </si>
+  <si>
+    <t>275536N</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>C623I</t>
+  </si>
+  <si>
+    <t>SAN BARTOLOME TIRAJANA, CUEVAS DEL PINAR</t>
+  </si>
+  <si>
+    <t>153600W</t>
+  </si>
+  <si>
+    <t>275125N</t>
+  </si>
+  <si>
+    <t>806</t>
+  </si>
+  <si>
+    <t>C625O</t>
+  </si>
+  <si>
+    <t>SAN BARTOLOME TIRAJANA, LOMOS PEDRO AFONSO</t>
+  </si>
+  <si>
+    <t>153842W</t>
+  </si>
+  <si>
+    <t>275432N</t>
+  </si>
+  <si>
+    <t>318</t>
+  </si>
+  <si>
+    <t>C628B</t>
+  </si>
+  <si>
+    <t>LA ALDEA DE SAN NICOLÁS, TASARTE</t>
+  </si>
+  <si>
+    <t>154612W</t>
+  </si>
+  <si>
+    <t>274648N</t>
+  </si>
+  <si>
+    <t>C629Q</t>
+  </si>
+  <si>
+    <t>MOGÁN, PUERTO RICO</t>
+  </si>
+  <si>
+    <t>154240W</t>
+  </si>
+  <si>
     <t>274859N</t>
   </si>
   <si>
@@ -817,6 +1261,81 @@
     <t>154551W</t>
   </si>
   <si>
+    <t>275512N</t>
+  </si>
+  <si>
+    <t>960</t>
+  </si>
+  <si>
+    <t>C635B</t>
+  </si>
+  <si>
+    <t>SAN BARTOLOME TIRAJANA, LAS TIRAJANAS</t>
+  </si>
+  <si>
+    <t>153427W</t>
+  </si>
+  <si>
+    <t>274529N</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>C639M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MASPALOMAS, C. INSULAR TURISMO </t>
+  </si>
+  <si>
+    <t>153432W</t>
+  </si>
+  <si>
+    <t>274845N</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>C639U</t>
+  </si>
+  <si>
+    <t>SAN BARTOLOME TIRAJANA, EL MATORRAL</t>
+  </si>
+  <si>
+    <t>152712W</t>
+  </si>
+  <si>
+    <t>275409N</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>C648C</t>
+  </si>
+  <si>
+    <t>AGÜIMES</t>
+  </si>
+  <si>
+    <t>152714W</t>
+  </si>
+  <si>
+    <t>275915N</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>C648N</t>
+  </si>
+  <si>
+    <t>TELDE, CENTRO FORESTAL DORAMAS</t>
+  </si>
+  <si>
+    <t>152728W</t>
+  </si>
+  <si>
     <t>275504N</t>
   </si>
   <si>
@@ -835,6 +1354,60 @@
     <t>152343W</t>
   </si>
   <si>
+    <t>275913N</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>C649R</t>
+  </si>
+  <si>
+    <t>TELDE, MELENARA</t>
+  </si>
+  <si>
+    <t>152240W</t>
+  </si>
+  <si>
+    <t>280431N</t>
+  </si>
+  <si>
+    <t>683</t>
+  </si>
+  <si>
+    <t>C656V</t>
+  </si>
+  <si>
+    <t>TEROR</t>
+  </si>
+  <si>
+    <t>153250W</t>
+  </si>
+  <si>
+    <t>280430N</t>
+  </si>
+  <si>
+    <t>269</t>
+  </si>
+  <si>
+    <t>C658L</t>
+  </si>
+  <si>
+    <t>LAS PALMAS DE G.C. (TAFIRA CMT)</t>
+  </si>
+  <si>
+    <t>152703W</t>
+  </si>
+  <si>
+    <t>280441N</t>
+  </si>
+  <si>
+    <t>C658X</t>
+  </si>
+  <si>
+    <t>LAS PALMAS DE GRAN CANARIA, TAFIRA</t>
+  </si>
+  <si>
     <t>55</t>
   </si>
   <si>
@@ -865,6 +1438,51 @@
     <t>152517W</t>
   </si>
   <si>
+    <t>280358N</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>C665T</t>
+  </si>
+  <si>
+    <t>VALLESECO</t>
+  </si>
+  <si>
+    <t>153357W</t>
+  </si>
+  <si>
+    <t>280540N</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t>C668V</t>
+  </si>
+  <si>
+    <t>AGAETE - SUERTE ALTA</t>
+  </si>
+  <si>
+    <t>154030W</t>
+  </si>
+  <si>
+    <t>280830N</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>C669B</t>
+  </si>
+  <si>
+    <t>ARUCAS</t>
+  </si>
+  <si>
+    <t>153025W</t>
+  </si>
+  <si>
     <t>274409N</t>
   </si>
   <si>
@@ -892,6 +1510,96 @@
     <t>133007W</t>
   </si>
   <si>
+    <t>291346N</t>
+  </si>
+  <si>
+    <t>C839X</t>
+  </si>
+  <si>
+    <t>LA GRACIOSA</t>
+  </si>
+  <si>
+    <t>60045</t>
+  </si>
+  <si>
+    <t>133037W</t>
+  </si>
+  <si>
+    <t>274308N</t>
+  </si>
+  <si>
+    <t>948</t>
+  </si>
+  <si>
+    <t>C916Q</t>
+  </si>
+  <si>
+    <t>EL PINAR, DEPÓSITO</t>
+  </si>
+  <si>
+    <t>175841W</t>
+  </si>
+  <si>
+    <t>274331N</t>
+  </si>
+  <si>
+    <t>715</t>
+  </si>
+  <si>
+    <t>C917E</t>
+  </si>
+  <si>
+    <t>EL PINAR, LA DEHESA</t>
+  </si>
+  <si>
+    <t>180654W</t>
+  </si>
+  <si>
+    <t>273955N</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>C919K</t>
+  </si>
+  <si>
+    <t>TACORON-LAPILLAS-TORTUGA</t>
+  </si>
+  <si>
+    <t>180107W</t>
+  </si>
+  <si>
+    <t>274607N</t>
+  </si>
+  <si>
+    <t>1070</t>
+  </si>
+  <si>
+    <t>C925F</t>
+  </si>
+  <si>
+    <t>SAN ANDRÉS, VALVERDE</t>
+  </si>
+  <si>
+    <t>175736W</t>
+  </si>
+  <si>
+    <t>274839N</t>
+  </si>
+  <si>
+    <t>670</t>
+  </si>
+  <si>
+    <t>C928I</t>
+  </si>
+  <si>
+    <t>VALVERDE</t>
+  </si>
+  <si>
+    <t>175510W</t>
+  </si>
+  <si>
     <t>274908N</t>
   </si>
   <si>
@@ -908,6 +1616,21 @@
   </si>
   <si>
     <t>175320W</t>
+  </si>
+  <si>
+    <t>274523N</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>C939T</t>
+  </si>
+  <si>
+    <t>FRONTERA, SABINOSA</t>
+  </si>
+  <si>
+    <t>180624W</t>
   </si>
 </sst>
 </file>
@@ -1270,20 +1993,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +2028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1326,7 +2048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +2091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1389,7 +2111,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1409,7 +2131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1429,7 +2151,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1449,7 +2171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1469,7 +2191,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1489,7 +2211,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1509,7 +2231,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1532,7 +2254,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1555,7 +2277,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1575,7 +2297,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1598,7 +2320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -1618,7 +2340,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1638,7 +2360,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -1661,7 +2383,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1681,7 +2403,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -1701,7 +2423,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -1721,7 +2443,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -1741,7 +2463,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>119</v>
       </c>
@@ -1761,7 +2483,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -1781,7 +2503,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -1804,7 +2526,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -1827,7 +2549,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -1847,7 +2569,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>144</v>
       </c>
@@ -1867,7 +2589,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -1887,7 +2609,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>155</v>
       </c>
@@ -1907,7 +2629,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>160</v>
       </c>
@@ -1927,7 +2649,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>165</v>
       </c>
@@ -1947,7 +2669,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>170</v>
       </c>
@@ -1967,7 +2689,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>175</v>
       </c>
@@ -1987,7 +2709,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>180</v>
       </c>
@@ -2007,7 +2729,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -2027,7 +2749,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>189</v>
       </c>
@@ -2047,7 +2769,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -2067,7 +2789,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>199</v>
       </c>
@@ -2087,7 +2809,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>204</v>
       </c>
@@ -2107,7 +2829,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>209</v>
       </c>
@@ -2127,7 +2849,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>214</v>
       </c>
@@ -2150,7 +2872,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>220</v>
       </c>
@@ -2173,7 +2895,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>226</v>
       </c>
@@ -2193,12 +2915,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>231</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
         <v>232</v>
@@ -2209,261 +2931,1250 @@
       <c r="E45" t="s">
         <v>234</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>235</v>
       </c>
-      <c r="G45" t="s">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" t="s">
         <v>237</v>
       </c>
-      <c r="B46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>238</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>239</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>240</v>
       </c>
-      <c r="F46" t="s">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>241</v>
-      </c>
-      <c r="G46" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>243</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
       </c>
       <c r="C47" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" t="s">
+        <v>243</v>
+      </c>
+      <c r="E47" t="s">
         <v>244</v>
       </c>
-      <c r="D47" t="s">
+      <c r="G47" t="s">
         <v>245</v>
       </c>
-      <c r="E47" t="s">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>246</v>
-      </c>
-      <c r="F47" t="s">
-        <v>247</v>
-      </c>
-      <c r="G47" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>249</v>
       </c>
       <c r="B48" t="s">
         <v>35</v>
       </c>
       <c r="C48" t="s">
+        <v>247</v>
+      </c>
+      <c r="D48" t="s">
+        <v>248</v>
+      </c>
+      <c r="E48" t="s">
+        <v>249</v>
+      </c>
+      <c r="F48" t="s">
+        <v>250</v>
+      </c>
+      <c r="G48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>252</v>
+      </c>
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" t="s">
+        <v>255</v>
+      </c>
+      <c r="G49" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>257</v>
+      </c>
+      <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" t="s">
+        <v>259</v>
+      </c>
+      <c r="E50" t="s">
+        <v>260</v>
+      </c>
+      <c r="F50" t="s">
+        <v>261</v>
+      </c>
+      <c r="G50" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>263</v>
+      </c>
+      <c r="B51" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" t="s">
+        <v>264</v>
+      </c>
+      <c r="D51" t="s">
+        <v>265</v>
+      </c>
+      <c r="E51" t="s">
+        <v>266</v>
+      </c>
+      <c r="G51" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>268</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" t="s">
+        <v>271</v>
+      </c>
+      <c r="F52" t="s">
+        <v>272</v>
+      </c>
+      <c r="G52" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>274</v>
+      </c>
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>275</v>
+      </c>
+      <c r="D53" t="s">
+        <v>276</v>
+      </c>
+      <c r="E53" t="s">
+        <v>277</v>
+      </c>
+      <c r="G53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" t="s">
+        <v>281</v>
+      </c>
+      <c r="E54" t="s">
+        <v>282</v>
+      </c>
+      <c r="G54" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>284</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" t="s">
+        <v>285</v>
+      </c>
+      <c r="D55" t="s">
+        <v>286</v>
+      </c>
+      <c r="E55" t="s">
+        <v>287</v>
+      </c>
+      <c r="G55" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>289</v>
+      </c>
+      <c r="B56" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" t="s">
+        <v>290</v>
+      </c>
+      <c r="D56" t="s">
+        <v>291</v>
+      </c>
+      <c r="E56" t="s">
+        <v>292</v>
+      </c>
+      <c r="G56" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>294</v>
+      </c>
+      <c r="B57" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" t="s">
+        <v>295</v>
+      </c>
+      <c r="D57" t="s">
+        <v>296</v>
+      </c>
+      <c r="E57" t="s">
+        <v>297</v>
+      </c>
+      <c r="G57" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>299</v>
+      </c>
+      <c r="B58" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" t="s">
+        <v>300</v>
+      </c>
+      <c r="D58" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" t="s">
+        <v>302</v>
+      </c>
+      <c r="G58" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>304</v>
+      </c>
+      <c r="B59" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" t="s">
+        <v>306</v>
+      </c>
+      <c r="E59" t="s">
+        <v>307</v>
+      </c>
+      <c r="G59" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>309</v>
+      </c>
+      <c r="B60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" t="s">
+        <v>310</v>
+      </c>
+      <c r="D60" t="s">
+        <v>311</v>
+      </c>
+      <c r="E60" t="s">
+        <v>312</v>
+      </c>
+      <c r="G60" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>314</v>
+      </c>
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>315</v>
+      </c>
+      <c r="D61" t="s">
+        <v>316</v>
+      </c>
+      <c r="E61" t="s">
+        <v>317</v>
+      </c>
+      <c r="G61" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>319</v>
+      </c>
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" t="s">
+        <v>320</v>
+      </c>
+      <c r="D62" t="s">
+        <v>321</v>
+      </c>
+      <c r="E62" t="s">
+        <v>322</v>
+      </c>
+      <c r="G62" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>324</v>
+      </c>
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" t="s">
+        <v>325</v>
+      </c>
+      <c r="D63" t="s">
+        <v>326</v>
+      </c>
+      <c r="E63" t="s">
+        <v>327</v>
+      </c>
+      <c r="G63" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>329</v>
+      </c>
+      <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" t="s">
         <v>94</v>
       </c>
-      <c r="D48" t="s">
-        <v>250</v>
-      </c>
-      <c r="E48" t="s">
-        <v>251</v>
-      </c>
-      <c r="F48" t="s">
-        <v>252</v>
-      </c>
-      <c r="G48" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>254</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="D64" t="s">
+        <v>330</v>
+      </c>
+      <c r="E64" t="s">
+        <v>331</v>
+      </c>
+      <c r="F64" t="s">
+        <v>332</v>
+      </c>
+      <c r="G64" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>334</v>
+      </c>
+      <c r="B65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" t="s">
+        <v>335</v>
+      </c>
+      <c r="D65" t="s">
+        <v>336</v>
+      </c>
+      <c r="E65" t="s">
+        <v>337</v>
+      </c>
+      <c r="G65" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>339</v>
+      </c>
+      <c r="B66" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" t="s">
+        <v>232</v>
+      </c>
+      <c r="D66" t="s">
+        <v>340</v>
+      </c>
+      <c r="E66" t="s">
+        <v>341</v>
+      </c>
+      <c r="G66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>343</v>
+      </c>
+      <c r="B67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" t="s">
+        <v>344</v>
+      </c>
+      <c r="D67" t="s">
+        <v>345</v>
+      </c>
+      <c r="E67" t="s">
+        <v>346</v>
+      </c>
+      <c r="G67" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>348</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
+        <v>349</v>
+      </c>
+      <c r="D68" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" t="s">
+        <v>351</v>
+      </c>
+      <c r="G68" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>353</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" t="s">
+        <v>354</v>
+      </c>
+      <c r="D69" t="s">
+        <v>355</v>
+      </c>
+      <c r="E69" t="s">
+        <v>356</v>
+      </c>
+      <c r="G69" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>358</v>
+      </c>
+      <c r="B70" t="s">
         <v>8</v>
       </c>
-      <c r="C49" t="s">
-        <v>255</v>
-      </c>
-      <c r="D49" t="s">
-        <v>256</v>
-      </c>
-      <c r="E49" t="s">
-        <v>257</v>
-      </c>
-      <c r="F49" t="s">
-        <v>258</v>
-      </c>
-      <c r="G49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>260</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C70" t="s">
+        <v>359</v>
+      </c>
+      <c r="D70" t="s">
+        <v>360</v>
+      </c>
+      <c r="E70" t="s">
+        <v>361</v>
+      </c>
+      <c r="G70" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>363</v>
+      </c>
+      <c r="B71" t="s">
         <v>8</v>
       </c>
-      <c r="C50" t="s">
-        <v>255</v>
-      </c>
-      <c r="D50" t="s">
-        <v>261</v>
-      </c>
-      <c r="E50" t="s">
-        <v>262</v>
-      </c>
-      <c r="F50" t="s">
-        <v>263</v>
-      </c>
-      <c r="G50" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>265</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C71" t="s">
+        <v>364</v>
+      </c>
+      <c r="D71" t="s">
+        <v>365</v>
+      </c>
+      <c r="E71" t="s">
+        <v>366</v>
+      </c>
+      <c r="G71" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>368</v>
+      </c>
+      <c r="B72" t="s">
         <v>8</v>
       </c>
-      <c r="C51" t="s">
-        <v>266</v>
-      </c>
-      <c r="D51" t="s">
-        <v>267</v>
-      </c>
-      <c r="E51" t="s">
-        <v>268</v>
-      </c>
-      <c r="F51" t="s">
-        <v>269</v>
-      </c>
-      <c r="G51" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="C72" t="s">
+        <v>369</v>
+      </c>
+      <c r="D72" t="s">
+        <v>370</v>
+      </c>
+      <c r="E72" t="s">
+        <v>371</v>
+      </c>
+      <c r="F72" t="s">
+        <v>372</v>
+      </c>
+      <c r="G72" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>374</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>375</v>
+      </c>
+      <c r="D73" t="s">
+        <v>376</v>
+      </c>
+      <c r="E73" t="s">
+        <v>377</v>
+      </c>
+      <c r="F73" t="s">
+        <v>378</v>
+      </c>
+      <c r="G73" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>380</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>381</v>
+      </c>
+      <c r="D74" t="s">
+        <v>382</v>
+      </c>
+      <c r="E74" t="s">
+        <v>383</v>
+      </c>
+      <c r="G74" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>385</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>386</v>
+      </c>
+      <c r="D75" t="s">
+        <v>387</v>
+      </c>
+      <c r="E75" t="s">
+        <v>377</v>
+      </c>
+      <c r="F75" t="s">
+        <v>378</v>
+      </c>
+      <c r="G75" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>389</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>390</v>
+      </c>
+      <c r="D76" t="s">
+        <v>391</v>
+      </c>
+      <c r="E76" t="s">
+        <v>392</v>
+      </c>
+      <c r="G76" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>394</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>395</v>
+      </c>
+      <c r="D77" t="s">
+        <v>396</v>
+      </c>
+      <c r="E77" t="s">
+        <v>397</v>
+      </c>
+      <c r="G77" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>399</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>400</v>
+      </c>
+      <c r="D78" t="s">
+        <v>401</v>
+      </c>
+      <c r="E78" t="s">
+        <v>402</v>
+      </c>
+      <c r="G78" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>404</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>375</v>
+      </c>
+      <c r="D79" t="s">
+        <v>405</v>
+      </c>
+      <c r="E79" t="s">
+        <v>406</v>
+      </c>
+      <c r="G79" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>408</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>375</v>
+      </c>
+      <c r="D80" t="s">
+        <v>409</v>
+      </c>
+      <c r="E80" t="s">
+        <v>410</v>
+      </c>
+      <c r="F80" t="s">
+        <v>411</v>
+      </c>
+      <c r="G80" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>413</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>414</v>
+      </c>
+      <c r="D81" t="s">
+        <v>415</v>
+      </c>
+      <c r="E81" t="s">
+        <v>416</v>
+      </c>
+      <c r="G81" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>418</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>419</v>
+      </c>
+      <c r="D82" t="s">
+        <v>420</v>
+      </c>
+      <c r="E82" t="s">
+        <v>421</v>
+      </c>
+      <c r="G82" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>423</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>424</v>
+      </c>
+      <c r="D83" t="s">
+        <v>425</v>
+      </c>
+      <c r="E83" t="s">
+        <v>426</v>
+      </c>
+      <c r="G83" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>428</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>429</v>
+      </c>
+      <c r="D84" t="s">
+        <v>430</v>
+      </c>
+      <c r="E84" t="s">
+        <v>431</v>
+      </c>
+      <c r="G84" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>433</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>434</v>
+      </c>
+      <c r="D85" t="s">
+        <v>435</v>
+      </c>
+      <c r="E85" t="s">
+        <v>436</v>
+      </c>
+      <c r="G85" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>438</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>439</v>
+      </c>
+      <c r="D86" t="s">
+        <v>440</v>
+      </c>
+      <c r="E86" t="s">
+        <v>441</v>
+      </c>
+      <c r="F86" t="s">
+        <v>442</v>
+      </c>
+      <c r="G86" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>444</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>445</v>
+      </c>
+      <c r="D87" t="s">
+        <v>446</v>
+      </c>
+      <c r="E87" t="s">
+        <v>447</v>
+      </c>
+      <c r="G87" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>449</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>450</v>
+      </c>
+      <c r="D88" t="s">
+        <v>451</v>
+      </c>
+      <c r="E88" t="s">
+        <v>452</v>
+      </c>
+      <c r="G88" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>454</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>455</v>
+      </c>
+      <c r="D89" t="s">
+        <v>456</v>
+      </c>
+      <c r="E89" t="s">
+        <v>457</v>
+      </c>
+      <c r="G89" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>459</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>455</v>
+      </c>
+      <c r="D90" t="s">
+        <v>460</v>
+      </c>
+      <c r="E90" t="s">
+        <v>461</v>
+      </c>
+      <c r="G90" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>134</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B91" t="s">
         <v>8</v>
       </c>
-      <c r="C52" t="s">
-        <v>271</v>
-      </c>
-      <c r="D52" t="s">
-        <v>272</v>
-      </c>
-      <c r="E52" t="s">
-        <v>273</v>
-      </c>
-      <c r="F52" t="s">
-        <v>274</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="C91" t="s">
+        <v>462</v>
+      </c>
+      <c r="D91" t="s">
+        <v>463</v>
+      </c>
+      <c r="E91" t="s">
+        <v>464</v>
+      </c>
+      <c r="F91" t="s">
+        <v>465</v>
+      </c>
+      <c r="G91" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>467</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" t="s">
+        <v>468</v>
+      </c>
+      <c r="E92" t="s">
+        <v>469</v>
+      </c>
+      <c r="F92" t="s">
+        <v>470</v>
+      </c>
+      <c r="G92" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>472</v>
+      </c>
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>473</v>
+      </c>
+      <c r="D93" t="s">
+        <v>474</v>
+      </c>
+      <c r="E93" t="s">
+        <v>475</v>
+      </c>
+      <c r="G93" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>477</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>478</v>
+      </c>
+      <c r="D94" t="s">
+        <v>479</v>
+      </c>
+      <c r="E94" t="s">
+        <v>480</v>
+      </c>
+      <c r="G94" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>482</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>483</v>
+      </c>
+      <c r="D95" t="s">
+        <v>484</v>
+      </c>
+      <c r="E95" t="s">
+        <v>485</v>
+      </c>
+      <c r="G95" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>487</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" t="s">
+        <v>488</v>
+      </c>
+      <c r="E96" t="s">
+        <v>489</v>
+      </c>
+      <c r="F96" t="s">
+        <v>490</v>
+      </c>
+      <c r="G96" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>492</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>375</v>
+      </c>
+      <c r="D97" t="s">
+        <v>493</v>
+      </c>
+      <c r="E97" t="s">
+        <v>494</v>
+      </c>
+      <c r="G97" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>496</v>
+      </c>
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>276</v>
-      </c>
-      <c r="B53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" t="s">
-        <v>78</v>
-      </c>
-      <c r="D53" t="s">
-        <v>277</v>
-      </c>
-      <c r="E53" t="s">
-        <v>278</v>
-      </c>
-      <c r="F53" t="s">
-        <v>279</v>
-      </c>
-      <c r="G53" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>281</v>
-      </c>
-      <c r="B54" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" t="s">
-        <v>282</v>
-      </c>
-      <c r="E54" t="s">
-        <v>283</v>
-      </c>
-      <c r="F54" t="s">
-        <v>284</v>
-      </c>
-      <c r="G54" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>286</v>
-      </c>
-      <c r="B55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>255</v>
-      </c>
-      <c r="D55" t="s">
-        <v>287</v>
-      </c>
-      <c r="E55" t="s">
-        <v>288</v>
-      </c>
-      <c r="G55" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>290</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="D98" t="s">
+        <v>497</v>
+      </c>
+      <c r="E98" t="s">
+        <v>498</v>
+      </c>
+      <c r="F98" t="s">
+        <v>499</v>
+      </c>
+      <c r="G98" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>501</v>
+      </c>
+      <c r="B99" t="s">
         <v>35</v>
       </c>
-      <c r="C56" t="s">
-        <v>291</v>
-      </c>
-      <c r="D56" t="s">
-        <v>292</v>
-      </c>
-      <c r="E56" t="s">
-        <v>293</v>
-      </c>
-      <c r="F56" t="s">
-        <v>294</v>
-      </c>
-      <c r="G56" t="s">
-        <v>295</v>
+      <c r="C99" t="s">
+        <v>502</v>
+      </c>
+      <c r="D99" t="s">
+        <v>503</v>
+      </c>
+      <c r="E99" t="s">
+        <v>504</v>
+      </c>
+      <c r="G99" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>506</v>
+      </c>
+      <c r="B100" t="s">
+        <v>35</v>
+      </c>
+      <c r="C100" t="s">
+        <v>507</v>
+      </c>
+      <c r="D100" t="s">
+        <v>508</v>
+      </c>
+      <c r="E100" t="s">
+        <v>509</v>
+      </c>
+      <c r="G100" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>511</v>
+      </c>
+      <c r="B101" t="s">
+        <v>145</v>
+      </c>
+      <c r="C101" t="s">
+        <v>512</v>
+      </c>
+      <c r="D101" t="s">
+        <v>513</v>
+      </c>
+      <c r="E101" t="s">
+        <v>514</v>
+      </c>
+      <c r="G101" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>516</v>
+      </c>
+      <c r="B102" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" t="s">
+        <v>517</v>
+      </c>
+      <c r="D102" t="s">
+        <v>518</v>
+      </c>
+      <c r="E102" t="s">
+        <v>519</v>
+      </c>
+      <c r="G102" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>521</v>
+      </c>
+      <c r="B103" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" t="s">
+        <v>522</v>
+      </c>
+      <c r="D103" t="s">
+        <v>523</v>
+      </c>
+      <c r="E103" t="s">
+        <v>524</v>
+      </c>
+      <c r="G103" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>526</v>
+      </c>
+      <c r="B104" t="s">
+        <v>35</v>
+      </c>
+      <c r="C104" t="s">
+        <v>527</v>
+      </c>
+      <c r="D104" t="s">
+        <v>528</v>
+      </c>
+      <c r="E104" t="s">
+        <v>529</v>
+      </c>
+      <c r="F104" t="s">
+        <v>530</v>
+      </c>
+      <c r="G104" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>532</v>
+      </c>
+      <c r="B105" t="s">
+        <v>35</v>
+      </c>
+      <c r="C105" t="s">
+        <v>533</v>
+      </c>
+      <c r="D105" t="s">
+        <v>534</v>
+      </c>
+      <c r="E105" t="s">
+        <v>535</v>
+      </c>
+      <c r="G105" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>